<commit_message>
update after change in website
</commit_message>
<xml_diff>
--- a/test_case_final.xlsx
+++ b/test_case_final.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Document\Quality Assurance (QA)\0. Internship Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Document\GitHub\Nepse_Alpha-Pytest-Framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2430748B-A023-40BC-BCAE-DD7BB586B524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4531E49D-3260-4572-B4D0-79D0472D3708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="316">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -2636,19 +2636,6 @@
     <t>TC_044</t>
   </si>
   <si>
-    <t>1&gt; Windows 11 Home v22631.3527
- 2&gt; Chrome v124.0.6367.79
-3&gt; Network Speed 200Mbps</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1&gt; Windows 11 Home v22631.3527 (PC)
-2&gt; Redmi Note 11 Pro (Android)
- 3&gt; Chrome v124.0.6367.79 (PC)
-4&gt; Brave 1.65.114, Chromium 124.0.6367.60 (Android)
-5&gt; 3&gt; Network Speed 200Mbps
-</t>
-  </si>
-  <si>
     <r>
       <t>1&gt; Launch Browser and Enter the 
 URL "</t>
@@ -2868,12 +2855,27 @@
   <si>
     <t>This test case checks if the footer links on the homepage is clickable and redirects to the correct page.</t>
   </si>
+  <si>
+    <t>1&gt; Windows 11 Home v22631.4037
+ 2&gt; Chrome Version 128.0.6613.85
+3&gt; Firefox Version 129.0.2
+4&gt; Edge Version 128.0.2739.42
+5&gt; Network Speed 200Mbps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1&gt; Windows 11 Home v22631.4037 (PC)
+2&gt; Redmi Note 11 Pro (Android)
+ 3&gt; Chrome  128.0.6613.85 (PC)
+4&gt; Brave 1.65.114, Chromium 124.0.6367.60 (Android)
+5&gt; 3&gt; Network Speed 200Mbps
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26">
+  <fonts count="25">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -3026,13 +3028,6 @@
       <family val="1"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -3166,7 +3161,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3267,11 +3262,8 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3512,10 +3504,10 @@
   <dimension ref="A1:AF1034"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="8" topLeftCell="E50" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="8" topLeftCell="B39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="L51" sqref="L51"/>
+      <selection pane="bottomRight" activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -3529,7 +3521,7 @@
     <col min="7" max="7" width="28.21875" customWidth="1"/>
     <col min="8" max="8" width="38.33203125" customWidth="1"/>
     <col min="9" max="9" width="23.21875" customWidth="1"/>
-    <col min="10" max="10" width="30.6640625" customWidth="1"/>
+    <col min="10" max="10" width="35" customWidth="1"/>
     <col min="11" max="12" width="13.44140625" customWidth="1"/>
     <col min="13" max="13" width="20.6640625" customWidth="1"/>
     <col min="14" max="14" width="17.33203125" customWidth="1"/>
@@ -3538,41 +3530,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="15.75" customHeight="1">
-      <c r="A1" s="39"/>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="39"/>
-      <c r="S1" s="39"/>
-      <c r="T1" s="39"/>
-      <c r="U1" s="39"/>
-      <c r="V1" s="39"/>
-      <c r="W1" s="39"/>
-      <c r="X1" s="39"/>
-      <c r="Y1" s="39"/>
-      <c r="Z1" s="39"/>
-      <c r="AA1" s="39"/>
-      <c r="AB1" s="39"/>
+      <c r="A1" s="38"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="38"/>
+      <c r="V1" s="38"/>
+      <c r="W1" s="38"/>
+      <c r="X1" s="38"/>
+      <c r="Y1" s="38"/>
+      <c r="Z1" s="38"/>
+      <c r="AA1" s="38"/>
+      <c r="AB1" s="38"/>
     </row>
     <row r="2" spans="1:32" ht="17.399999999999999">
       <c r="A2" s="3"/>
       <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="35" t="s">
         <v>26</v>
       </c>
       <c r="E2" s="6"/>
@@ -3875,7 +3867,7 @@
         <v>23</v>
       </c>
       <c r="J9" s="25" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="K9" s="22" t="s">
         <v>16</v>
@@ -3887,7 +3879,7 @@
       <c r="N9" s="28" t="s">
         <v>269</v>
       </c>
-      <c r="O9" s="35" t="s">
+      <c r="O9" s="33" t="s">
         <v>199</v>
       </c>
       <c r="P9" s="34" t="s">
@@ -3910,7 +3902,7 @@
       <c r="AE9" s="2"/>
       <c r="AF9" s="2"/>
     </row>
-    <row r="10" spans="1:32" ht="78" customHeight="1">
+    <row r="10" spans="1:32" ht="78">
       <c r="A10" s="3"/>
       <c r="B10" s="22" t="s">
         <v>21</v>
@@ -3937,7 +3929,7 @@
         <v>23</v>
       </c>
       <c r="J10" s="25" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="K10" s="22" t="s">
         <v>16</v>
@@ -3995,7 +3987,7 @@
         <v>23</v>
       </c>
       <c r="J11" s="25" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="K11" s="22" t="s">
         <v>16</v>
@@ -4053,7 +4045,7 @@
         <v>23</v>
       </c>
       <c r="J12" s="25" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="K12" s="22" t="s">
         <v>16</v>
@@ -4111,7 +4103,7 @@
         <v>23</v>
       </c>
       <c r="J13" s="25" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="K13" s="22" t="s">
         <v>16</v>
@@ -4169,7 +4161,7 @@
         <v>23</v>
       </c>
       <c r="J14" s="25" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="K14" s="22" t="s">
         <v>16</v>
@@ -4227,7 +4219,7 @@
         <v>23</v>
       </c>
       <c r="J15" s="25" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="K15" s="22" t="s">
         <v>16</v>
@@ -4285,7 +4277,7 @@
         <v>23</v>
       </c>
       <c r="J16" s="25" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="K16" s="22" t="s">
         <v>16</v>
@@ -4341,7 +4333,7 @@
         <v>23</v>
       </c>
       <c r="J17" s="25" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="K17" s="23" t="s">
         <v>16</v>
@@ -4390,16 +4382,16 @@
         <v>138</v>
       </c>
       <c r="G18" s="25" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="H18" s="25" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="I18" s="22" t="s">
         <v>23</v>
       </c>
       <c r="J18" s="25" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="K18" s="23"/>
       <c r="L18" s="22"/>
@@ -4455,7 +4447,7 @@
         <v>23</v>
       </c>
       <c r="J19" s="25" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="K19" s="23" t="s">
         <v>16</v>
@@ -4510,10 +4502,10 @@
         <v>97</v>
       </c>
       <c r="I20" s="25" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="J20" s="25" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="K20" s="23" t="s">
         <v>90</v>
@@ -4575,7 +4567,7 @@
         <v>23</v>
       </c>
       <c r="J21" s="25" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="K21" s="23" t="s">
         <v>16</v>
@@ -4630,15 +4622,15 @@
         <v>158</v>
       </c>
       <c r="I22" s="25" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="J22" s="25" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="K22" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="L22" s="37" t="s">
+      <c r="L22" s="36" t="s">
         <v>95</v>
       </c>
       <c r="M22" s="28" t="s">
@@ -4695,7 +4687,7 @@
         <v>23</v>
       </c>
       <c r="J23" s="25" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="K23" s="23" t="s">
         <v>16</v>
@@ -4753,7 +4745,7 @@
         <v>23</v>
       </c>
       <c r="J24" s="25" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="K24" s="23" t="s">
         <v>16</v>
@@ -4811,7 +4803,7 @@
         <v>23</v>
       </c>
       <c r="J25" s="25" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="K25" s="22" t="s">
         <v>16</v>
@@ -4869,7 +4861,7 @@
         <v>23</v>
       </c>
       <c r="J26" s="25" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="K26" s="23" t="s">
         <v>16</v>
@@ -4927,7 +4919,7 @@
         <v>23</v>
       </c>
       <c r="J27" s="25" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="K27" s="23" t="s">
         <v>16</v>
@@ -4985,7 +4977,7 @@
         <v>23</v>
       </c>
       <c r="J28" s="25" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="K28" s="23" t="s">
         <v>16</v>
@@ -5043,7 +5035,7 @@
         <v>23</v>
       </c>
       <c r="J29" s="25" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="K29" s="23" t="s">
         <v>16</v>
@@ -5101,7 +5093,7 @@
         <v>23</v>
       </c>
       <c r="J30" s="25" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="K30" s="23" t="s">
         <v>16</v>
@@ -5159,7 +5151,7 @@
         <v>23</v>
       </c>
       <c r="J31" s="25" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="K31" s="23" t="s">
         <v>16</v>
@@ -5217,7 +5209,7 @@
         <v>23</v>
       </c>
       <c r="J32" s="25" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="K32" s="23" t="s">
         <v>16</v>
@@ -5275,7 +5267,7 @@
         <v>23</v>
       </c>
       <c r="J33" s="25" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="K33" s="23" t="s">
         <v>16</v>
@@ -5333,7 +5325,7 @@
         <v>23</v>
       </c>
       <c r="J34" s="25" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="K34" s="23" t="s">
         <v>16</v>
@@ -5393,7 +5385,7 @@
         <v>23</v>
       </c>
       <c r="J35" s="25" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="K35" s="23" t="s">
         <v>16</v>
@@ -5453,7 +5445,7 @@
         <v>23</v>
       </c>
       <c r="J36" s="25" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="K36" s="23" t="s">
         <v>16</v>
@@ -5511,7 +5503,7 @@
         <v>23</v>
       </c>
       <c r="J37" s="25" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="K37" s="23" t="s">
         <v>16</v>
@@ -5542,7 +5534,7 @@
       <c r="AE37" s="2"/>
       <c r="AF37" s="2"/>
     </row>
-    <row r="38" spans="1:32" ht="156">
+    <row r="38" spans="1:32" ht="124.8">
       <c r="A38" s="3"/>
       <c r="B38" s="22" t="s">
         <v>108</v>
@@ -5566,16 +5558,16 @@
         <v>155</v>
       </c>
       <c r="I38" s="25" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="J38" s="25" t="s">
-        <v>297</v>
+        <v>315</v>
       </c>
       <c r="K38" s="23" t="s">
         <v>90</v>
       </c>
       <c r="L38" s="33" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="M38" s="28" t="s">
         <v>271</v>
@@ -5631,7 +5623,7 @@
         <v>23</v>
       </c>
       <c r="J39" s="25" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="K39" s="23" t="s">
         <v>16</v>
@@ -5689,7 +5681,7 @@
         <v>23</v>
       </c>
       <c r="J40" s="25" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="K40" s="23" t="s">
         <v>16</v>
@@ -5743,23 +5735,25 @@
       <c r="H41" s="25" t="s">
         <v>130</v>
       </c>
-      <c r="I41" s="22" t="s">
-        <v>23</v>
+      <c r="I41" s="25" t="s">
+        <v>299</v>
       </c>
       <c r="J41" s="25" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="K41" s="23" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="L41" s="22"/>
       <c r="M41" s="28" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="N41" s="28" t="s">
-        <v>269</v>
-      </c>
-      <c r="O41" s="23"/>
+        <v>91</v>
+      </c>
+      <c r="O41" s="33" t="s">
+        <v>199</v>
+      </c>
       <c r="P41" s="23"/>
       <c r="Q41" s="2"/>
       <c r="R41" s="2"/>
@@ -5805,7 +5799,7 @@
         <v>23</v>
       </c>
       <c r="J42" s="25" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="K42" s="23" t="s">
         <v>16</v>
@@ -5819,7 +5813,7 @@
       </c>
       <c r="O42" s="23"/>
       <c r="P42" s="24" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="Q42" s="2"/>
       <c r="R42" s="2"/>
@@ -5865,13 +5859,13 @@
         <v>166</v>
       </c>
       <c r="J43" s="25" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="K43" s="23" t="s">
         <v>90</v>
       </c>
       <c r="L43" s="33" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="M43" s="28" t="s">
         <v>271</v>
@@ -5917,23 +5911,23 @@
       <c r="F44" s="25" t="s">
         <v>277</v>
       </c>
-      <c r="G44" s="38" t="s">
-        <v>313</v>
+      <c r="G44" s="37" t="s">
+        <v>311</v>
       </c>
       <c r="H44" s="25" t="s">
         <v>278</v>
       </c>
       <c r="I44" s="25" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="J44" s="25" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="K44" s="23" t="s">
         <v>90</v>
       </c>
       <c r="L44" s="33" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="M44" s="28" t="s">
         <v>271</v>
@@ -5979,23 +5973,23 @@
       <c r="F45" s="25" t="s">
         <v>291</v>
       </c>
-      <c r="G45" s="38" t="s">
-        <v>313</v>
+      <c r="G45" s="37" t="s">
+        <v>311</v>
       </c>
       <c r="H45" s="25" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="I45" s="25" t="s">
         <v>292</v>
       </c>
       <c r="J45" s="25" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="K45" s="23" t="s">
         <v>90</v>
       </c>
       <c r="L45" s="33" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="M45" s="28" t="s">
         <v>271</v>
@@ -6042,7 +6036,7 @@
         <v>283</v>
       </c>
       <c r="G46" s="25" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="H46" s="25" t="s">
         <v>284</v>
@@ -6051,7 +6045,7 @@
         <v>285</v>
       </c>
       <c r="J46" s="25" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="K46" s="23" t="s">
         <v>16</v>
@@ -6094,10 +6088,10 @@
         <v>273</v>
       </c>
       <c r="E47" s="25" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F47" s="25" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G47" s="25"/>
       <c r="H47" s="25" t="s">
@@ -6107,13 +6101,13 @@
         <v>276</v>
       </c>
       <c r="J47" s="25" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="K47" s="23" t="s">
         <v>90</v>
       </c>
       <c r="L47" s="33" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="M47" s="28" t="s">
         <v>270</v>
@@ -6169,13 +6163,13 @@
         <v>166</v>
       </c>
       <c r="J48" s="25" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="K48" s="23" t="s">
         <v>90</v>
       </c>
       <c r="L48" s="33" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="M48" s="28" t="s">
         <v>270</v>
@@ -6231,13 +6225,13 @@
         <v>166</v>
       </c>
       <c r="J49" s="25" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="K49" s="23" t="s">
         <v>90</v>
       </c>
       <c r="L49" s="33" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="M49" s="28" t="s">
         <v>270</v>
@@ -6293,13 +6287,13 @@
         <v>166</v>
       </c>
       <c r="J50" s="25" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="K50" s="23" t="s">
         <v>90</v>
       </c>
       <c r="L50" s="33" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="M50" s="28" t="s">
         <v>270</v>
@@ -6337,7 +6331,7 @@
         <v>187</v>
       </c>
       <c r="D51" s="25" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E51" s="25" t="s">
         <v>192</v>
@@ -6355,7 +6349,7 @@
         <v>23</v>
       </c>
       <c r="J51" s="25" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="K51" s="23" t="s">
         <v>16</v>
@@ -6413,7 +6407,7 @@
         <v>23</v>
       </c>
       <c r="J52" s="25" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="K52" s="23" t="s">
         <v>16</v>
@@ -39872,17 +39866,17 @@
     <hyperlink ref="F11" r:id="rId17" display="https://www.nepsealpha.com/" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
     <hyperlink ref="F9" r:id="rId18" display="https://www.nepsealpha.com/" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
     <hyperlink ref="P9" r:id="rId19" display="https://shorturl.at/7BCqd" xr:uid="{FB734F31-FEA3-4695-8B62-C1FDE8914893}"/>
-    <hyperlink ref="O9" r:id="rId20" xr:uid="{B70BF940-C959-48F5-8801-8F03EF66B210}"/>
-    <hyperlink ref="O20" r:id="rId21" xr:uid="{25DFDA47-D6B3-4CF6-9B6C-0F9F8CC6A29C}"/>
-    <hyperlink ref="O43" r:id="rId22" xr:uid="{13898004-BEDA-4E08-9A86-27215A2E3DA6}"/>
-    <hyperlink ref="O47" r:id="rId23" xr:uid="{E7CA0A47-635D-4B01-8876-D645111A97EA}"/>
-    <hyperlink ref="O44" r:id="rId24" xr:uid="{E9D8A032-4064-4437-B485-486FBF993F6E}"/>
-    <hyperlink ref="O45" r:id="rId25" xr:uid="{638859F9-0C6A-4CE7-BFA7-E30E87D50D4E}"/>
-    <hyperlink ref="O48" r:id="rId26" xr:uid="{0EDCCCA9-5B22-4EF3-8197-FA5C5192BA98}"/>
-    <hyperlink ref="O49" r:id="rId27" xr:uid="{42DC749C-2440-4E30-90FE-4167C5091992}"/>
-    <hyperlink ref="O50" r:id="rId28" xr:uid="{4B917C94-41E3-485B-AB99-6FB99B8293E4}"/>
-    <hyperlink ref="O22" r:id="rId29" xr:uid="{EF6C92B4-F151-4855-8FEB-D40575ABDD38}"/>
-    <hyperlink ref="O38" r:id="rId30" xr:uid="{2ED6D495-F10F-46DF-83FD-7886572C281A}"/>
+    <hyperlink ref="O9" r:id="rId20" location="LTKmgHfNa2Tc" xr:uid="{B70BF940-C959-48F5-8801-8F03EF66B210}"/>
+    <hyperlink ref="O20" r:id="rId21" location="JAbCiH0p6LnN" xr:uid="{25DFDA47-D6B3-4CF6-9B6C-0F9F8CC6A29C}"/>
+    <hyperlink ref="O43" r:id="rId22" location="qD9ZWd7AVRrV" xr:uid="{13898004-BEDA-4E08-9A86-27215A2E3DA6}"/>
+    <hyperlink ref="O47" r:id="rId23" location="wfX9Fhys4dZ4" xr:uid="{E7CA0A47-635D-4B01-8876-D645111A97EA}"/>
+    <hyperlink ref="O44" r:id="rId24" location="EU3T9orFsd3Y" xr:uid="{E9D8A032-4064-4437-B485-486FBF993F6E}"/>
+    <hyperlink ref="O45" r:id="rId25" location="m8dE9402Iwhr" xr:uid="{638859F9-0C6A-4CE7-BFA7-E30E87D50D4E}"/>
+    <hyperlink ref="O48" r:id="rId26" location="9Jg76BXrRTSZ" xr:uid="{0EDCCCA9-5B22-4EF3-8197-FA5C5192BA98}"/>
+    <hyperlink ref="O49" r:id="rId27" location="sU4f6z6qXfow" xr:uid="{42DC749C-2440-4E30-90FE-4167C5091992}"/>
+    <hyperlink ref="O50" r:id="rId28" location="kmuU3XyOW9Pp" xr:uid="{4B917C94-41E3-485B-AB99-6FB99B8293E4}"/>
+    <hyperlink ref="O22" r:id="rId29" location="5croxShN8fNr" xr:uid="{EF6C92B4-F151-4855-8FEB-D40575ABDD38}"/>
+    <hyperlink ref="O38" r:id="rId30" location="JWn42NfElHYb" xr:uid="{2ED6D495-F10F-46DF-83FD-7886572C281A}"/>
     <hyperlink ref="D2" r:id="rId31" xr:uid="{B4B4CFCF-6EF8-4EFD-B4BB-651E4DB94DF9}"/>
     <hyperlink ref="L20" r:id="rId32" xr:uid="{595C561C-4E73-4BCF-A5DD-23C1888AFB39}"/>
     <hyperlink ref="L22" r:id="rId33" xr:uid="{A5FAA778-822A-4C66-9E02-7AF72A1BB7CA}"/>
@@ -39894,8 +39888,9 @@
     <hyperlink ref="L48" r:id="rId39" xr:uid="{78513355-37FE-4954-B998-84654A24A945}"/>
     <hyperlink ref="L49" r:id="rId40" xr:uid="{F0B6EB85-D1F6-455F-9695-1A8A934E7970}"/>
     <hyperlink ref="L50" r:id="rId41" xr:uid="{DB05FD99-EA6B-459A-BBDE-096FDE0CFF4E}"/>
+    <hyperlink ref="O41" r:id="rId42" location="egJAZ1QNtEKo" xr:uid="{31A6C642-2946-4C6F-942E-E93432535D9E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId42"/>
+  <pageSetup orientation="portrait" r:id="rId43"/>
 </worksheet>
 </file>
</xml_diff>